<commit_message>
Excel paralelo a modelo/import
</commit_message>
<xml_diff>
--- a/core/tests/maestro.xlsx
+++ b/core/tests/maestro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basededatos\Desarrollo\alphaGvame\alpha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basededatos\Desarrollo\alphaGvame\alpha\core\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
   <si>
     <t>Periodo</t>
   </si>
@@ -422,24 +422,12 @@
     <t>Carnet entregar</t>
   </si>
   <si>
-    <t>Telefono fixo</t>
-  </si>
-  <si>
-    <t>Telefono movil</t>
-  </si>
-  <si>
-    <t>Dni autorizado</t>
-  </si>
-  <si>
     <t>Tarjeta sanitaria</t>
   </si>
   <si>
     <t>Foto</t>
   </si>
   <si>
-    <t>Lopd</t>
-  </si>
-  <si>
     <t>Cuota socio</t>
   </si>
   <si>
@@ -447,6 +435,21 @@
   </si>
   <si>
     <t>Carnet entregado</t>
+  </si>
+  <si>
+    <t>Teléfono fixo</t>
+  </si>
+  <si>
+    <t>Teléfono movil</t>
+  </si>
+  <si>
+    <t>DNI autorizado</t>
+  </si>
+  <si>
+    <t>LOPD</t>
+  </si>
+  <si>
+    <t>Estado</t>
   </si>
 </sst>
 </file>
@@ -822,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -928,6 +931,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1210,15 +1219,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="A4" sqref="A4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="1" t="s">
@@ -1242,7 +1251,7 @@
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="1" t="s">
@@ -1264,7 +1273,7 @@
       <c r="O2" s="39"/>
       <c r="P2" s="39"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1282,11 +1291,11 @@
       <c r="O3" s="39"/>
       <c r="P3" s="39"/>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1297,40 +1306,43 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1372,7 +1384,7 @@
       </c>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1422,7 +1434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1460,7 +1472,7 @@
       </c>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1510,7 +1522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1554,7 +1566,7 @@
       </c>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1592,7 +1604,7 @@
       <c r="O10" s="24"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1630,7 +1642,7 @@
       </c>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1678,7 +1690,7 @@
       </c>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
@@ -1722,7 +1734,7 @@
       </c>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1768,7 +1780,7 @@
       </c>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1812,7 @@
       <c r="O15" s="19"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
cambia en excel IdFamilia por UIDMembresia
</commit_message>
<xml_diff>
--- a/core/tests/maestro.xlsx
+++ b/core/tests/maestro.xlsx
@@ -89,9 +89,6 @@
     <t>IdUsuario</t>
   </si>
   <si>
-    <t>IdFamilia</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -450,6 +447,9 @@
   </si>
   <si>
     <t>Estado</t>
+  </si>
+  <si>
+    <t>UIDMembresia</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1222,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:Q4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,67 +1296,67 @@
         <v>4</v>
       </c>
       <c r="B4" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="K4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="N4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q4" s="49" t="s">
         <v>124</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q4" s="49" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="25" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>13</v>
       </c>
       <c r="F5" s="14">
         <v>555856954</v>
@@ -1365,14 +1365,14 @@
         <v>555695232</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5">
@@ -1380,25 +1380,25 @@
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="14">
         <v>555856954</v>
@@ -1407,19 +1407,19 @@
         <v>555695232</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" s="17">
         <v>40</v>
@@ -1428,27 +1428,27 @@
         <v>40</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="14">
         <v>555856954</v>
@@ -1457,7 +1457,7 @@
         <v>555965235</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1468,25 +1468,25 @@
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="14">
         <v>555856954</v>
@@ -1495,19 +1495,19 @@
         <v>555789623</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8" s="17">
         <v>40</v>
@@ -1516,27 +1516,27 @@
         <v>0</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="F9" s="5">
         <v>555632222</v>
@@ -1545,14 +1545,14 @@
         <v>555632565</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5">
@@ -1562,42 +1562,42 @@
         <v>0</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>33</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
         <v>555978546</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K10" s="23"/>
       <c r="L10" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
@@ -1606,16 +1606,16 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>36</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="14">
@@ -1625,12 +1625,12 @@
         <v>555964786</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5">
@@ -1638,25 +1638,25 @@
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="14">
         <v>555666444</v>
@@ -1665,19 +1665,19 @@
         <v>555786547</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M12" s="5">
         <v>40</v>
@@ -1686,25 +1686,25 @@
         <v>40</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="14">
         <v>555666444</v>
@@ -1713,61 +1713,61 @@
         <v>555632147</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>48</v>
-      </c>
       <c r="D14" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="14">
         <v>555223145</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M14" s="5">
         <v>25</v>
@@ -1776,22 +1776,22 @@
         <v>25</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>51</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1814,16 +1814,16 @@
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>54</v>
-      </c>
       <c r="D16" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27">
@@ -1833,10 +1833,10 @@
         <v>22233555</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
@@ -1850,16 +1850,16 @@
     </row>
     <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5">
@@ -1869,7 +1869,7 @@
         <v>333666222</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1884,38 +1884,38 @@
     </row>
     <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="20" t="s">
+      <c r="D18" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="17">
         <v>222666333</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M18" s="23">
         <v>40</v>
@@ -1924,44 +1924,44 @@
         <v>40</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="D19" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>65</v>
-      </c>
       <c r="E19" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="14">
         <v>555999666</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" s="5">
         <v>40</v>
@@ -1970,25 +1970,25 @@
         <v>0</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="5">
         <v>222666999</v>
@@ -1997,7 +1997,7 @@
         <v>555333666</v>
       </c>
       <c r="H20" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -2012,19 +2012,19 @@
     </row>
     <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>71</v>
-      </c>
       <c r="D21" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="14">
         <v>555666444</v>
@@ -2033,19 +2033,19 @@
         <v>222222333</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M21" s="5">
         <v>54</v>
@@ -2056,16 +2056,16 @@
     </row>
     <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="D22" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="5">
@@ -2075,7 +2075,7 @@
         <v>211122233</v>
       </c>
       <c r="H22" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -2090,16 +2090,16 @@
     </row>
     <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5">
@@ -2109,7 +2109,7 @@
         <v>333666555</v>
       </c>
       <c r="H23" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -2120,25 +2120,25 @@
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>80</v>
-      </c>
       <c r="D24" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24" s="30">
         <v>666999333</v>
@@ -2147,19 +2147,19 @@
         <v>555333222</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L24" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M24" s="31">
         <v>40</v>
@@ -2168,25 +2168,25 @@
         <v>40</v>
       </c>
       <c r="O24" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="C25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" s="5">
         <v>332655441</v>
@@ -2195,7 +2195,7 @@
         <v>222555333</v>
       </c>
       <c r="H25" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -2206,69 +2206,69 @@
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="D26" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>84</v>
-      </c>
       <c r="E26" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="21">
         <v>333222111</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K26" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M26" s="23">
         <v>0</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="D27" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>84</v>
-      </c>
       <c r="E27" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="21">
         <v>333222111</v>
@@ -2277,19 +2277,19 @@
         <v>222333111</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M27" s="17">
         <v>40</v>
@@ -2298,22 +2298,22 @@
         <v>40</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="D28" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="14"/>
@@ -2321,7 +2321,7 @@
         <v>222666333</v>
       </c>
       <c r="H28" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2336,19 +2336,19 @@
     </row>
     <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="D29" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29" s="21">
         <v>333222111</v>
@@ -2357,7 +2357,7 @@
         <v>222666333</v>
       </c>
       <c r="H29" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2368,32 +2368,32 @@
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="D30" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>101</v>
-      </c>
       <c r="E30" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30" s="17">
         <v>222555333</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
@@ -2406,19 +2406,19 @@
     </row>
     <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>104</v>
-      </c>
       <c r="D31" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="36">
         <v>555222333</v>
@@ -2427,19 +2427,19 @@
         <v>333111444</v>
       </c>
       <c r="H31" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M31" s="5">
         <v>40</v>
@@ -2448,27 +2448,27 @@
         <v>40</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>107</v>
-      </c>
       <c r="D32" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="14">
         <v>555666444</v>
@@ -2477,12 +2477,12 @@
         <v>256322145</v>
       </c>
       <c r="H32" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5">
@@ -2490,39 +2490,39 @@
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>110</v>
-      </c>
       <c r="D33" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23">
         <v>232221452</v>
       </c>
       <c r="H33" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
       <c r="K33" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L33" s="23"/>
       <c r="M33" s="23">
@@ -2530,24 +2530,24 @@
       </c>
       <c r="N33" s="23"/>
       <c r="O33" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>113</v>
-      </c>
       <c r="D34" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="21">
@@ -2557,7 +2557,7 @@
         <v>298565474</v>
       </c>
       <c r="H34" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="23"/>

</xml_diff>

<commit_message>
Rellana campo Estado en Excel maestro
</commit_message>
<xml_diff>
--- a/core/tests/maestro.xlsx
+++ b/core/tests/maestro.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="128">
   <si>
     <t>Periodo</t>
   </si>
@@ -450,13 +450,19 @@
   </si>
   <si>
     <t>UIDMembresia</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +531,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -825,7 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -938,6 +951,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1221,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,6 +1399,9 @@
         <v>14</v>
       </c>
       <c r="P5" s="5"/>
+      <c r="Q5" s="50" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1432,6 +1451,9 @@
       </c>
       <c r="P6" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="Q6" s="51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1471,6 +1493,9 @@
         <v>14</v>
       </c>
       <c r="P7" s="5"/>
+      <c r="Q7" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1521,6 +1546,9 @@
       <c r="P8" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="Q8" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1565,6 +1593,9 @@
         <v>14</v>
       </c>
       <c r="P9" s="5"/>
+      <c r="Q9" s="50" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1603,6 +1634,9 @@
       <c r="N10" s="23"/>
       <c r="O10" s="24"/>
       <c r="P10" s="5"/>
+      <c r="Q10" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1641,6 +1675,9 @@
         <v>14</v>
       </c>
       <c r="P11" s="5"/>
+      <c r="Q11" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1689,6 +1726,9 @@
         <v>19</v>
       </c>
       <c r="P12" s="5"/>
+      <c r="Q12" s="52" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1733,6 +1773,9 @@
         <v>14</v>
       </c>
       <c r="P13" s="5"/>
+      <c r="Q13" s="52" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1779,6 +1822,9 @@
         <v>14</v>
       </c>
       <c r="P14" s="5"/>
+      <c r="Q14" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1811,6 +1857,9 @@
       <c r="N15" s="5"/>
       <c r="O15" s="19"/>
       <c r="P15" s="5"/>
+      <c r="Q15" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1847,8 +1896,11 @@
       <c r="N16" s="17"/>
       <c r="O16" s="18"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q16" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1881,8 +1933,11 @@
       <c r="N17" s="5"/>
       <c r="O17" s="19"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q17" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -1927,8 +1982,11 @@
         <v>19</v>
       </c>
       <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q18" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
@@ -1973,8 +2031,11 @@
         <v>14</v>
       </c>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q19" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
@@ -2009,8 +2070,11 @@
       <c r="N20" s="5"/>
       <c r="O20" s="19"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q20" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>69</v>
       </c>
@@ -2053,8 +2117,11 @@
       <c r="N21" s="5"/>
       <c r="O21" s="19"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q21" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>72</v>
       </c>
@@ -2087,8 +2154,11 @@
       <c r="N22" s="17"/>
       <c r="O22" s="19"/>
       <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q22" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>75</v>
       </c>
@@ -2123,8 +2193,11 @@
         <v>19</v>
       </c>
       <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q23" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>78</v>
       </c>
@@ -2171,8 +2244,11 @@
         <v>14</v>
       </c>
       <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q24" s="52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>81</v>
       </c>
@@ -2209,8 +2285,11 @@
         <v>85</v>
       </c>
       <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q25" s="52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>86</v>
       </c>
@@ -2253,8 +2332,11 @@
         <v>19</v>
       </c>
       <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q26" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>89</v>
       </c>
@@ -2301,8 +2383,11 @@
         <v>14</v>
       </c>
       <c r="P27" s="5"/>
-    </row>
-    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q27" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -2333,8 +2418,11 @@
       <c r="N28" s="5"/>
       <c r="O28" s="19"/>
       <c r="P28" s="5"/>
-    </row>
-    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q28" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>95</v>
       </c>
@@ -2371,8 +2459,11 @@
         <v>85</v>
       </c>
       <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q29" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>97</v>
       </c>
@@ -2403,8 +2494,11 @@
       <c r="N30" s="17"/>
       <c r="O30" s="18"/>
       <c r="P30" s="5"/>
-    </row>
-    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q30" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>102</v>
       </c>
@@ -2453,8 +2547,11 @@
       <c r="P31" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q31" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>105</v>
       </c>
@@ -2495,8 +2592,11 @@
       <c r="P32" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q32" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>108</v>
       </c>
@@ -2535,8 +2635,11 @@
       <c r="P33" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q33" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>111</v>
       </c>
@@ -2569,6 +2672,9 @@
       <c r="N34" s="23"/>
       <c r="O34" s="24"/>
       <c r="P34" s="5"/>
+      <c r="Q34" s="52" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
añada una familia más
</commit_message>
<xml_diff>
--- a/core/tests/maestro.xlsx
+++ b/core/tests/maestro.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="135">
   <si>
     <t>Periodo</t>
   </si>
@@ -375,6 +375,60 @@
   </si>
   <si>
     <t>marville@gmail.com</t>
+  </si>
+  <si>
+    <t>dcc0af9c-b7d1-46be-ab41-4ba3132ddfc8</t>
+  </si>
+  <si>
+    <t>191c4842-0fee-425c-88b9-3429b3d55c3e</t>
+  </si>
+  <si>
+    <t>388da00f-75dc-4237-8095-159fb36c9ef7</t>
+  </si>
+  <si>
+    <t>894ed7f7-abda-445f-81fa-27c4354f3972</t>
+  </si>
+  <si>
+    <t>84237503-bb90-4287-9b26-1f311a7a557f</t>
+  </si>
+  <si>
+    <t>c238d560-e629-4b48-8863-611b8c7beb4f</t>
+  </si>
+  <si>
+    <t>b20d04ca-acaa-44b2-8fd7-f7a9422164eb</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Álvarez Álvarez</t>
+  </si>
+  <si>
+    <t>Joven García</t>
+  </si>
+  <si>
+    <t>Joven Álvarez</t>
+  </si>
+  <si>
+    <t>Xabier</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Alma</t>
+  </si>
+  <si>
+    <t>marjo@gmail.com</t>
+  </si>
+  <si>
+    <t>salav@gmail.com</t>
+  </si>
+  <si>
+    <t>rogarjo@arquitectos.com</t>
+  </si>
+  <si>
+    <t>almajo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1332,9 @@
       <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="M5" s="5">
         <v>40</v>
       </c>
@@ -1472,7 +1528,9 @@
       <c r="K9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="17" t="s">
@@ -1915,7 +1973,9 @@
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="K19" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="L19" s="15"/>
       <c r="M19" s="5">
         <v>40</v>
@@ -1923,8 +1983,12 @@
       <c r="N19" s="5">
         <v>40</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="5"/>
+      <c r="O19" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="Q19" s="41" t="s">
         <v>55</v>
       </c>
@@ -2201,7 +2265,9 @@
         <v>15</v>
       </c>
       <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
+      <c r="O25" s="43" t="s">
+        <v>11</v>
+      </c>
       <c r="P25" s="43"/>
       <c r="Q25" s="41" t="s">
         <v>55</v>
@@ -2295,6 +2361,288 @@
         <v>55</v>
       </c>
     </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G28" s="43">
+        <v>664455445</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="43">
+        <v>40</v>
+      </c>
+      <c r="N28" s="43">
+        <v>40</v>
+      </c>
+      <c r="O28" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="P28" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q28" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G29" s="43">
+        <v>664455445</v>
+      </c>
+      <c r="H29" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G30" s="43">
+        <v>699664556</v>
+      </c>
+      <c r="H30" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="P30" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G31" s="43">
+        <v>664455445</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q31" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G32" s="43">
+        <v>664455445</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="I32" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="43">
+        <v>986662448</v>
+      </c>
+      <c r="G33" s="43">
+        <v>698545698</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="I33" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modifica el importdata y el excel para que se asignen los grupos a los destinatarios
</commit_message>
<xml_diff>
--- a/core/tests/maestro.xlsx
+++ b/core/tests/maestro.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basededatos\Desarrollo\alphaGvame\alpha\core\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estefy\Desktop\proyecto_abertal\alpha\core\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="usuarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="136">
   <si>
     <t>Periodo</t>
   </si>
@@ -429,12 +429,15 @@
   </si>
   <si>
     <t>almajo@gmail.com</t>
+  </si>
+  <si>
+    <t>Destinatario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -678,19 +681,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -727,15 +717,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -782,12 +763,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -820,9 +812,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -832,37 +821,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -878,14 +860,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1167,25 +1158,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="C30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1193,23 +1184,24 @@
         <v>1</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,41 +1209,43 @@
         <v>305</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-    </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="34" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1260,45 +1254,48 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="39" t="s">
+      <c r="R4" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1308,42 +1305,45 @@
       <c r="C5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="21">
         <v>986223332</v>
       </c>
-      <c r="G5" s="24">
+      <c r="H5" s="22">
         <v>662193321</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="I5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5">
-        <v>40</v>
-      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="5">
         <v>40</v>
       </c>
-      <c r="O5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="40" t="s">
+      <c r="O5" s="5">
+        <v>40</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1353,46 +1353,49 @@
       <c r="C6" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="21">
         <v>986223332</v>
       </c>
-      <c r="G6" s="24">
+      <c r="H6" s="22">
         <v>662193321</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="I6" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="41" t="s">
+      <c r="J6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1402,44 +1405,47 @@
       <c r="C7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="21">
         <v>986223332</v>
       </c>
-      <c r="G7" s="17">
+      <c r="H7" s="16">
         <v>665442312</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="I7" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="J7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="41" t="s">
+      <c r="O7" s="5"/>
+      <c r="P7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -1449,46 +1455,49 @@
       <c r="C8" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="21">
         <v>986223332</v>
       </c>
-      <c r="G8" s="17">
+      <c r="H8" s="16">
         <v>663193556</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="I8" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="41" t="s">
+      <c r="J8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1498,65 +1507,68 @@
       <c r="C9" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="42">
         <v>986223332</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>663193556</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="40" t="s">
+      <c r="O9" s="5"/>
+      <c r="P9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="21">
         <v>986334443</v>
       </c>
-      <c r="G10" s="20">
+      <c r="H10" s="18">
         <v>618881118</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="I10" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="J10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1566,62 +1578,68 @@
       <c r="L10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="5">
-        <v>40</v>
+      <c r="M10" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="N10" s="5">
         <v>40</v>
       </c>
-      <c r="O10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="41" t="s">
+      <c r="O10" s="5">
+        <v>40</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="21">
         <v>986334443</v>
       </c>
-      <c r="G11" s="24">
+      <c r="H11" s="22">
         <v>618881118</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="I11" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="41" t="s">
+      <c r="O11" s="5"/>
+      <c r="P11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1631,1003 +1649,1069 @@
       <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="21">
         <v>986334443</v>
       </c>
-      <c r="G12" s="24">
+      <c r="H12" s="22">
         <v>618881118</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="I12" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="41" t="s">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="21">
         <v>986442224</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="14">
         <v>655436661</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="I13" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="J13" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="5">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="N13" s="5">
         <v>15</v>
       </c>
-      <c r="O13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="41" t="s">
+      <c r="O13" s="5">
+        <v>15</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="12">
         <v>986663336</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>669432214</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="I14" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5">
-        <v>40</v>
-      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="5"/>
       <c r="N14" s="5">
         <v>40</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="5">
+        <v>40</v>
+      </c>
+      <c r="P14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="41" t="s">
+      <c r="Q14" s="5"/>
+      <c r="R14" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="12">
         <v>986663336</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="5">
         <v>669432214</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="I15" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="41" t="s">
+      <c r="J15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12">
         <v>986663336</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>669432214</v>
       </c>
-      <c r="H16" s="43" t="s">
+      <c r="I16" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="40" t="s">
+      <c r="J16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" s="36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="16" t="s">
         <v>81</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="12">
         <v>986663336</v>
       </c>
-      <c r="G17" s="5">
+      <c r="H17" s="5">
         <v>669432214</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="I17" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="5"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="42" t="s">
+      <c r="O17" s="5"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="16" t="s">
         <v>83</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="12">
         <v>986663336</v>
       </c>
-      <c r="G18" s="15">
+      <c r="H18" s="14">
         <v>667778899</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="5"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="14"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="5"/>
+      <c r="P18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="41" t="s">
+      <c r="Q18" s="5"/>
+      <c r="R18" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="27" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="27">
         <v>986323445</v>
       </c>
-      <c r="G19" s="15">
+      <c r="H19" s="14">
         <v>621151515</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="I19" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="5">
-        <v>40</v>
-      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="14"/>
       <c r="N19" s="5">
         <v>40</v>
       </c>
-      <c r="O19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="41" t="s">
+      <c r="O19" s="5">
+        <v>40</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="27">
         <v>986323445</v>
       </c>
-      <c r="G20" s="15">
+      <c r="H20" s="14">
         <v>621151515</v>
       </c>
-      <c r="H20" s="43" t="s">
+      <c r="I20" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="J20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M20" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="N20" s="5"/>
-      <c r="O20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q20" s="40" t="s">
+      <c r="O20" s="5"/>
+      <c r="P20" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="12">
         <v>986445876</v>
       </c>
-      <c r="G21" s="32">
+      <c r="H21" s="29">
         <v>662443998</v>
       </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="33"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21" s="41" t="s">
+      <c r="O21" s="5"/>
+      <c r="P21" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="27">
         <v>986323445</v>
       </c>
-      <c r="G22" s="21">
+      <c r="H22" s="19">
         <v>664338833</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>95</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q22" s="41" t="s">
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="27">
         <v>986323445</v>
       </c>
-      <c r="G23" s="15">
+      <c r="H23" s="14">
         <v>621151515</v>
       </c>
-      <c r="H23" s="43" t="s">
+      <c r="I23" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="I23" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="41" t="s">
+      <c r="J23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="47">
         <v>986434445</v>
       </c>
-      <c r="G24" s="43">
+      <c r="H24" s="39">
         <v>655411886</v>
       </c>
-      <c r="H24" s="43" t="s">
+      <c r="I24" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" s="43">
+      <c r="J24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="39">
         <v>15</v>
       </c>
-      <c r="N24" s="43">
+      <c r="O24" s="39">
         <v>15</v>
       </c>
-      <c r="O24" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="41" t="s">
+      <c r="P24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="47">
         <v>986334668</v>
       </c>
-      <c r="G25" s="43">
+      <c r="H25" s="39">
         <v>664879621</v>
       </c>
-      <c r="H25" s="43" t="s">
+      <c r="I25" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M25" s="43">
+      <c r="J25" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="39">
         <v>15</v>
       </c>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="41" t="s">
+      <c r="O25" s="39"/>
+      <c r="P25" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43">
+      <c r="F26" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="47"/>
+      <c r="H26" s="39">
         <v>625125521</v>
       </c>
-      <c r="H26" s="43" t="s">
+      <c r="I26" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="46" t="s">
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="47">
         <v>986554369</v>
       </c>
-      <c r="G27" s="43">
+      <c r="H27" s="39">
         <v>665442332</v>
       </c>
-      <c r="H27" s="43" t="s">
+      <c r="I27" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="I27" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" s="43">
+      <c r="J27" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="39">
         <v>15</v>
       </c>
-      <c r="N27" s="43">
+      <c r="O27" s="39">
         <v>15</v>
       </c>
-      <c r="O27" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P27" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q27" s="41" t="s">
+      <c r="P27" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q27" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R27" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="E28" s="43" t="s">
+      <c r="E28" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="47">
         <v>986662448</v>
       </c>
-      <c r="G28" s="43">
+      <c r="H28" s="39">
         <v>664455445</v>
       </c>
-      <c r="H28" s="43" t="s">
+      <c r="I28" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="I28" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M28" s="43">
+      <c r="J28" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="39">
         <v>40</v>
       </c>
-      <c r="N28" s="43">
+      <c r="O28" s="39">
         <v>40</v>
       </c>
-      <c r="O28" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P28" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q28" s="41" t="s">
+      <c r="P28" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q28" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E29" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="47">
         <v>986662448</v>
       </c>
-      <c r="G29" s="43">
+      <c r="H29" s="39">
         <v>664455445</v>
       </c>
-      <c r="H29" s="43" t="s">
+      <c r="I29" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P29" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q29" s="41" t="s">
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q29" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R29" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="E30" s="43" t="s">
+      <c r="E30" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="47">
         <v>986662448</v>
       </c>
-      <c r="G30" s="43">
+      <c r="H30" s="39">
         <v>699664556</v>
       </c>
-      <c r="H30" s="43" t="s">
+      <c r="I30" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P30" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q30" s="41" t="s">
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q30" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R30" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F31" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="47">
         <v>986662448</v>
       </c>
-      <c r="G31" s="43">
+      <c r="H31" s="39">
         <v>664455445</v>
       </c>
-      <c r="H31" s="43" t="s">
+      <c r="I31" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="I31" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K31" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="P31" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q31" s="41" t="s">
+      <c r="J31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R31" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="43" t="s">
+      <c r="E32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="43">
+      <c r="F32" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="47">
         <v>986662448</v>
       </c>
-      <c r="G32" s="43">
+      <c r="H32" s="39">
         <v>664455445</v>
       </c>
-      <c r="H32" s="43" t="s">
+      <c r="I32" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="I32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="41" t="s">
+      <c r="J32" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="43">
+      <c r="F33" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="47">
         <v>986662448</v>
       </c>
-      <c r="G33" s="43">
+      <c r="H33" s="39">
         <v>698545698</v>
       </c>
-      <c r="H33" s="43" t="s">
+      <c r="I33" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="I33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="41" t="s">
+      <c r="J33" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="37" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>